<commit_message>
preserve energy for the with/without filter cases
</commit_message>
<xml_diff>
--- a/results/compareCIFAR-10-PytorchPreserveEnergy.xlsx
+++ b/results/compareCIFAR-10-PytorchPreserveEnergy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\time-series-machine-leaning\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE8349A-D5A0-4DD8-852F-5A42542A0223}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C80D93-B7B2-4AB4-A5B1-72C7EF2F18A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" activeTab="2" xr2:uid="{6B079C5B-DCCE-420F-B497-C9CB4E3D061F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" activeTab="1" xr2:uid="{6B079C5B-DCCE-420F-B497-C9CB4E3D061F}"/>
   </bookViews>
   <sheets>
     <sheet name="energy100" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,12 +130,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2651,7 +2667,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2830,6 +2846,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2837,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679FE752-A557-453C-8A87-17247EEC7967}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3017,6 +3034,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3024,7 +3042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB77310-A71B-47D5-BFDB-41A17FE2B8FB}">
   <dimension ref="A2:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3122,94 +3140,95 @@
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+      <c r="A3" s="1">
         <f>energy100!A4</f>
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f>energy100!$E4</f>
         <v>32.5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>energy90!$E4</f>
         <v>28.61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+      <c r="A4" s="1">
         <f>energy100!A5</f>
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <f>energy100!$E5</f>
         <v>35.92</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>energy90!$E5</f>
         <v>33.57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+      <c r="A5" s="1">
         <f>energy100!A6</f>
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f>energy100!$E6</f>
         <v>39.869999999999997</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>energy90!$E6</f>
         <v>35.01</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="A6" s="1">
         <f>energy100!A7</f>
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <f>energy100!$E7</f>
         <v>45.24</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <f>energy90!$E7</f>
         <v>34.39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+      <c r="A7" s="1">
         <f>energy100!A8</f>
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <f>energy100!$E8</f>
         <v>43.41</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <f>energy90!$E8</f>
         <v>34.29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
check index back and preserved energy
</commit_message>
<xml_diff>
--- a/results/compareCIFAR-10-PytorchPreserveEnergy.xlsx
+++ b/results/compareCIFAR-10-PytorchPreserveEnergy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\time-series-machine-leaning\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C80D93-B7B2-4AB4-A5B1-72C7EF2F18A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0932500F-247A-4ADA-B8F8-857BF5D0FB72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" activeTab="1" xr2:uid="{6B079C5B-DCCE-420F-B497-C9CB4E3D061F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="8412" activeTab="2" xr2:uid="{6B079C5B-DCCE-420F-B497-C9CB4E3D061F}"/>
   </bookViews>
   <sheets>
     <sheet name="energy100" sheetId="1" r:id="rId1"/>
@@ -271,10 +271,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>compareTrain!$B$3:$B$7</c:f>
+              <c:f>compareTrain!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>36.411999999999999</c:v>
                 </c:pt>
@@ -289,6 +289,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>46.954000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.167999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.573999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.287999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.042000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51.326000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -325,10 +340,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>compareTrain!$C$3:$C$7</c:f>
+              <c:f>compareTrain!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>32.058</c:v>
                 </c:pt>
@@ -343,6 +358,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>40.682000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.932000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.481999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.661999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41.167999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.103999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,8 +766,8 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>compareTest!$B$2</c:f>
@@ -745,84 +775,6 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>energy100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>compareTest!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>compareTest!$B$3:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>32.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35.92</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>39.869999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45.24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.41</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4E8F-4C3A-8010-C4FE8A133EAF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>compareTest!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>energy90</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -837,50 +789,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>compareTest!$A$3:$A$7</c:f>
+              <c:f>compareTest!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>35.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>39.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>45.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>compareTest!$C$3:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>28.61</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>33.57</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35.01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.39</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34.29</c:v>
+                  <c:v>43.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49.56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,6 +831,75 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4E8F-4C3A-8010-C4FE8A133EAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>compareTest!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>energy90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>compareTest!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>28.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.119999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.770000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-28AE-4A3C-8F88-70D81D92B843}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -903,6 +915,93 @@
         <c:overlap val="-27"/>
         <c:axId val="323687072"/>
         <c:axId val="236908640"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>compareTest!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>epoch</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>compareTest!$A$3:$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-4E8F-4C3A-8010-C4FE8A133EAF}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="323687072"/>
@@ -2664,10 +2763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469FC407-17D8-4C1D-B47D-708320C8EA35}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2842,6 +2941,106 @@
       </c>
       <c r="F8">
         <v>17876.586283922101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1.4363794883728001</v>
+      </c>
+      <c r="C9">
+        <v>49.167999999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.5443183504104601</v>
+      </c>
+      <c r="E9">
+        <v>46.22</v>
+      </c>
+      <c r="F9">
+        <v>17877.3597483634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1.3706269609069801</v>
+      </c>
+      <c r="C10">
+        <v>52.573999999999998</v>
+      </c>
+      <c r="D10">
+        <v>1.4903003274917599</v>
+      </c>
+      <c r="E10">
+        <v>48.93</v>
+      </c>
+      <c r="F10">
+        <v>17877.112397670699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1.34872302871704</v>
+      </c>
+      <c r="C11">
+        <v>53.287999999999997</v>
+      </c>
+      <c r="D11">
+        <v>1.45679516925811</v>
+      </c>
+      <c r="E11">
+        <v>49.56</v>
+      </c>
+      <c r="F11">
+        <v>17878.0991001129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1.3774120434570301</v>
+      </c>
+      <c r="C12">
+        <v>52.042000000000002</v>
+      </c>
+      <c r="D12">
+        <v>1.5124543636322001</v>
+      </c>
+      <c r="E12">
+        <v>48.95</v>
+      </c>
+      <c r="F12">
+        <v>17877.3807842731</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1.3746770053100501</v>
+      </c>
+      <c r="C13">
+        <v>51.326000000000001</v>
+      </c>
+      <c r="D13">
+        <v>1.50309035739898</v>
+      </c>
+      <c r="E13">
+        <v>48.94</v>
+      </c>
+      <c r="F13">
+        <v>17876.807709455399</v>
       </c>
     </row>
   </sheetData>
@@ -2852,10 +3051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679FE752-A557-453C-8A87-17247EEC7967}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3030,6 +3229,106 @@
       </c>
       <c r="F8">
         <v>18285.443978071198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1.7067696926879801</v>
+      </c>
+      <c r="C9">
+        <v>36.932000000000002</v>
+      </c>
+      <c r="D9">
+        <v>1.8401764753341601</v>
+      </c>
+      <c r="E9">
+        <v>35.229999999999997</v>
+      </c>
+      <c r="F9">
+        <v>18287.223980188301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1.65963431213378</v>
+      </c>
+      <c r="C10">
+        <v>40.481999999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.8936904756546</v>
+      </c>
+      <c r="E10">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="F10">
+        <v>18288.388278961102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1.61274944946289</v>
+      </c>
+      <c r="C11">
+        <v>42.661999999999999</v>
+      </c>
+      <c r="D11">
+        <v>1.8255511009216301</v>
+      </c>
+      <c r="E11">
+        <v>35.82</v>
+      </c>
+      <c r="F11">
+        <v>18289.271656036301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1.63180855377197</v>
+      </c>
+      <c r="C12">
+        <v>41.167999999999999</v>
+      </c>
+      <c r="D12">
+        <v>1.8477833881378101</v>
+      </c>
+      <c r="E12">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="F12">
+        <v>18290.788039684201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1.56732403778076</v>
+      </c>
+      <c r="C13">
+        <v>44.103999999999999</v>
+      </c>
+      <c r="D13">
+        <v>1.8773306785583399</v>
+      </c>
+      <c r="E13">
+        <v>36.1</v>
+      </c>
+      <c r="F13">
+        <v>18292.2441513538</v>
       </c>
     </row>
   </sheetData>
@@ -3040,10 +3339,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB77310-A71B-47D5-BFDB-41A17FE2B8FB}">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3127,6 +3426,76 @@
       <c r="C7">
         <f>energy90!$C8</f>
         <v>40.682000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <f>energy100!A9</f>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>energy100!$C9</f>
+        <v>49.167999999999999</v>
+      </c>
+      <c r="C8">
+        <f>energy90!$C9</f>
+        <v>36.932000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <f>energy100!A10</f>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f>energy100!$C10</f>
+        <v>52.573999999999998</v>
+      </c>
+      <c r="C9">
+        <f>energy90!$C10</f>
+        <v>40.481999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <f>energy100!A11</f>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f>energy100!$C11</f>
+        <v>53.287999999999997</v>
+      </c>
+      <c r="C10">
+        <f>energy90!$C11</f>
+        <v>42.661999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <f>energy100!A12</f>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>energy100!$C12</f>
+        <v>52.042000000000002</v>
+      </c>
+      <c r="C11">
+        <f>energy90!$C12</f>
+        <v>41.167999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <f>energy100!A13</f>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>energy100!$C13</f>
+        <v>51.326000000000001</v>
+      </c>
+      <c r="C12">
+        <f>energy90!$C13</f>
+        <v>44.103999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3137,10 +3506,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A89391C-8F67-40DA-BF62-D84EA2914DF5}">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3226,6 +3595,76 @@
         <v>34.29</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
+        <f>energy100!A9</f>
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <f>energy100!$E9</f>
+        <v>46.22</v>
+      </c>
+      <c r="C8" s="1">
+        <f>energy90!$E9</f>
+        <v>35.229999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1">
+        <f>energy100!A10</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <f>energy100!$E10</f>
+        <v>48.93</v>
+      </c>
+      <c r="C9" s="1">
+        <f>energy90!$E10</f>
+        <v>35.119999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
+        <f>energy100!A11</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <f>energy100!$E11</f>
+        <v>49.56</v>
+      </c>
+      <c r="C10" s="1">
+        <f>energy90!$E11</f>
+        <v>35.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1">
+        <f>energy100!A12</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <f>energy100!$E12</f>
+        <v>48.95</v>
+      </c>
+      <c r="C11" s="1">
+        <f>energy90!$E12</f>
+        <v>34.770000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
+        <f>energy100!A13</f>
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <f>energy100!$E13</f>
+        <v>48.94</v>
+      </c>
+      <c r="C12" s="1">
+        <f>energy90!$E13</f>
+        <v>36.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>